<commit_message>
added looney tunes script
</commit_message>
<xml_diff>
--- a/ButtonMappings.xlsx
+++ b/ButtonMappings.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\PiNoiseBox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D01DA94-2C74-4687-969A-3272F3DC94BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219A747B-1064-48A4-B9DB-4D3C3917476C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03F1238B-2121-4505-ADD8-E9D055959FBB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{03F1238B-2121-4505-ADD8-E9D055959FBB}"/>
   </bookViews>
   <sheets>
     <sheet name="SoundFx" sheetId="1" r:id="rId1"/>
+    <sheet name="LooneyTunes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="122">
   <si>
     <t>aoogah.wav</t>
   </si>
@@ -279,6 +280,126 @@
   </si>
   <si>
     <t>Play</t>
+  </si>
+  <si>
+    <t>bugs_goodbye.wav</t>
+  </si>
+  <si>
+    <t>bugs_here_i_come.wav</t>
+  </si>
+  <si>
+    <t>bugs_whats_up_doc.wav</t>
+  </si>
+  <si>
+    <t>chicken_hawk.wav</t>
+  </si>
+  <si>
+    <t>daffy_are_u_nuts.wav</t>
+  </si>
+  <si>
+    <t>daffy_cut_that_out.wav</t>
+  </si>
+  <si>
+    <t>daffy_despicable.wav</t>
+  </si>
+  <si>
+    <t>elmer_be_very_quiet.wav</t>
+  </si>
+  <si>
+    <t>elmer_come_back.wav</t>
+  </si>
+  <si>
+    <t>elmer_hunting.wav</t>
+  </si>
+  <si>
+    <t>elmer_screwy.wav</t>
+  </si>
+  <si>
+    <t>marvin_angry.wav</t>
+  </si>
+  <si>
+    <t>marvin_bit_nice.wav</t>
+  </si>
+  <si>
+    <t>porky_thats_all_folks.wav</t>
+  </si>
+  <si>
+    <t>roadrunner2.wav</t>
+  </si>
+  <si>
+    <t>sylvester_sufferin.wav</t>
+  </si>
+  <si>
+    <t>taz.wav</t>
+  </si>
+  <si>
+    <t>tweety_bad2.wav</t>
+  </si>
+  <si>
+    <t>tweety_puddy_tat.wav</t>
+  </si>
+  <si>
+    <t>yosemite_toads.wav</t>
+  </si>
+  <si>
+    <t>bugs_goodbye</t>
+  </si>
+  <si>
+    <t>bugs_here_i_come</t>
+  </si>
+  <si>
+    <t>bugs_whats_up_doc</t>
+  </si>
+  <si>
+    <t>chicken_hawk</t>
+  </si>
+  <si>
+    <t>daffy_are_u_nuts</t>
+  </si>
+  <si>
+    <t>daffy_cut_that_out</t>
+  </si>
+  <si>
+    <t>daffy_despicable</t>
+  </si>
+  <si>
+    <t>elmer_be_very_quiet</t>
+  </si>
+  <si>
+    <t>elmer_come_back</t>
+  </si>
+  <si>
+    <t>elmer_hunting</t>
+  </si>
+  <si>
+    <t>elmer_screwy</t>
+  </si>
+  <si>
+    <t>marvin_angry</t>
+  </si>
+  <si>
+    <t>marvin_bit_nice</t>
+  </si>
+  <si>
+    <t>porky_thats_all_folks</t>
+  </si>
+  <si>
+    <t>roadrunner2</t>
+  </si>
+  <si>
+    <t>sylvester_sufferin</t>
+  </si>
+  <si>
+    <t>taz</t>
+  </si>
+  <si>
+    <t>tweety_bad2</t>
+  </si>
+  <si>
+    <t>tweety_puddy_tat</t>
+  </si>
+  <si>
+    <t>yosemite_toads</t>
   </si>
 </sst>
 </file>
@@ -353,6 +474,33 @@
       <calculatedColumnFormula>CONCATENATE(B2," = pygame.mixer.Sound(",CHAR(34),D2,CHAR(34),")")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{138A49E7-B7E4-43C6-ACF7-F99ACBAB6095}" name="Play">
+      <calculatedColumnFormula>CONCATENATE(A2,".when_pressed = ",B2,".play")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{94F39493-37C5-4317-8A50-3C3E7B9F9132}" name="Table22" displayName="Table22" ref="A1:F21" totalsRowShown="0">
+  <autoFilter ref="A1:F21" xr:uid="{50035476-F1BE-46DD-AC95-193826D5210C}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{6CBA259B-1807-41B7-90E9-17B0EC27B2E7}" name="Button"/>
+    <tableColumn id="2" xr3:uid="{807A7340-BC79-46AC-AFA8-3A76E68383DD}" name="BaseName"/>
+    <tableColumn id="3" xr3:uid="{80310CD7-D0FD-47A7-BEA1-39BE91CC9569}" name="FileName"/>
+    <tableColumn id="4" xr3:uid="{4C7C5679-D294-4C59-98EA-49AA9A74FFED}" name="Path">
+      <calculatedColumnFormula>CONCATENATE("/gpio-soundboard/soundfx/",C2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{F458A734-C51D-4BB4-B8F9-D932C756992A}" name="PythonCode">
+      <calculatedColumnFormula>CONCATENATE(B2," = pygame.mixer.Sound(",CHAR(34),D2,CHAR(34),")")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5B85D947-DDB3-4C14-BCEE-EAAFD10D9F31}" name="Play">
       <calculatedColumnFormula>CONCATENATE(A2,".when_pressed = ",B2,".play")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -659,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C2AB5-7878-4B8D-AD4F-E78907393A96}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1318,4 +1466,509 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5000B9D1-FDBD-428F-B14F-DD492970F2F0}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.88671875" customWidth="1"/>
+    <col min="5" max="5" width="93.33203125" customWidth="1"/>
+    <col min="6" max="6" width="38.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C2)</f>
+        <v>/gpio-soundboard/looneytunes/bugs_goodbye.wav</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE(B2," = pygame.mixer.Sound(",CHAR(34),D2,CHAR(34),")")</f>
+        <v>bugs_goodbye = pygame.mixer.Sound("/gpio-soundboard/looneytunes/bugs_goodbye.wav")</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE(A2,".when_pressed = ",B2,".play")</f>
+        <v>btn2.when_pressed = bugs_goodbye.play</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C3)</f>
+        <v>/gpio-soundboard/looneytunes/bugs_here_i_come.wav</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E21" si="0">CONCATENATE(B3," = pygame.mixer.Sound(",CHAR(34),D3,CHAR(34),")")</f>
+        <v>bugs_here_i_come = pygame.mixer.Sound("/gpio-soundboard/looneytunes/bugs_here_i_come.wav")</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F21" si="1">CONCATENATE(A3,".when_pressed = ",B3,".play")</f>
+        <v>btn3.when_pressed = bugs_here_i_come.play</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C4)</f>
+        <v>/gpio-soundboard/looneytunes/bugs_whats_up_doc.wav</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>bugs_whats_up_doc = pygame.mixer.Sound("/gpio-soundboard/looneytunes/bugs_whats_up_doc.wav")</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>btn15.when_pressed = bugs_whats_up_doc.play</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C5)</f>
+        <v>/gpio-soundboard/looneytunes/chicken_hawk.wav</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>chicken_hawk = pygame.mixer.Sound("/gpio-soundboard/looneytunes/chicken_hawk.wav")</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>btn27.when_pressed = chicken_hawk.play</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C6)</f>
+        <v>/gpio-soundboard/looneytunes/daffy_are_u_nuts.wav</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>daffy_are_u_nuts = pygame.mixer.Sound("/gpio-soundboard/looneytunes/daffy_are_u_nuts.wav")</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>btn22.when_pressed = daffy_are_u_nuts.play</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C7)</f>
+        <v>/gpio-soundboard/looneytunes/daffy_cut_that_out.wav</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>daffy_cut_that_out = pygame.mixer.Sound("/gpio-soundboard/looneytunes/daffy_cut_that_out.wav")</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>btn23.when_pressed = daffy_cut_that_out.play</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C8)</f>
+        <v>/gpio-soundboard/looneytunes/daffy_despicable.wav</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>daffy_despicable = pygame.mixer.Sound("/gpio-soundboard/looneytunes/daffy_despicable.wav")</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>btn25.when_pressed = daffy_despicable.play</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C9)</f>
+        <v>/gpio-soundboard/looneytunes/elmer_be_very_quiet.wav</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>elmer_be_very_quiet = pygame.mixer.Sound("/gpio-soundboard/looneytunes/elmer_be_very_quiet.wav")</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>btn5.when_pressed = elmer_be_very_quiet.play</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C10)</f>
+        <v>/gpio-soundboard/looneytunes/elmer_come_back.wav</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>elmer_come_back = pygame.mixer.Sound("/gpio-soundboard/looneytunes/elmer_come_back.wav")</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>btn21.when_pressed = elmer_come_back.play</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C11)</f>
+        <v>/gpio-soundboard/looneytunes/elmer_hunting.wav</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>elmer_hunting = pygame.mixer.Sound("/gpio-soundboard/looneytunes/elmer_hunting.wav")</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>btn12.when_pressed = elmer_hunting.play</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C12)</f>
+        <v>/gpio-soundboard/looneytunes/elmer_screwy.wav</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>elmer_screwy = pygame.mixer.Sound("/gpio-soundboard/looneytunes/elmer_screwy.wav")</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>btn13.when_pressed = elmer_screwy.play</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C13)</f>
+        <v>/gpio-soundboard/looneytunes/marvin_angry.wav</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>marvin_angry = pygame.mixer.Sound("/gpio-soundboard/looneytunes/marvin_angry.wav")</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>btn16.when_pressed = marvin_angry.play</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C14)</f>
+        <v>/gpio-soundboard/looneytunes/marvin_bit_nice.wav</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>marvin_bit_nice = pygame.mixer.Sound("/gpio-soundboard/looneytunes/marvin_bit_nice.wav")</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>btn20.when_pressed = marvin_bit_nice.play</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C15)</f>
+        <v>/gpio-soundboard/looneytunes/porky_thats_all_folks.wav</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>porky_thats_all_folks = pygame.mixer.Sound("/gpio-soundboard/looneytunes/porky_thats_all_folks.wav")</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>btn19.when_pressed = porky_thats_all_folks.play</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C16)</f>
+        <v>/gpio-soundboard/looneytunes/roadrunner2.wav</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>roadrunner2 = pygame.mixer.Sound("/gpio-soundboard/looneytunes/roadrunner2.wav")</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>btn26.when_pressed = roadrunner2.play</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C17)</f>
+        <v>/gpio-soundboard/looneytunes/sylvester_sufferin.wav</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>sylvester_sufferin = pygame.mixer.Sound("/gpio-soundboard/looneytunes/sylvester_sufferin.wav")</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>btn18.when_pressed = sylvester_sufferin.play</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C18)</f>
+        <v>/gpio-soundboard/looneytunes/taz.wav</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>taz = pygame.mixer.Sound("/gpio-soundboard/looneytunes/taz.wav")</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>btn14.when_pressed = taz.play</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C19)</f>
+        <v>/gpio-soundboard/looneytunes/tweety_bad2.wav</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>tweety_bad2 = pygame.mixer.Sound("/gpio-soundboard/looneytunes/tweety_bad2.wav")</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>btn6.when_pressed = tweety_bad2.play</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C20)</f>
+        <v>/gpio-soundboard/looneytunes/tweety_puddy_tat.wav</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>tweety_puddy_tat = pygame.mixer.Sound("/gpio-soundboard/looneytunes/tweety_puddy_tat.wav")</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>btn4.when_pressed = tweety_puddy_tat.play</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" t="str">
+        <f>CONCATENATE("/gpio-soundboard/looneytunes/",C21)</f>
+        <v>/gpio-soundboard/looneytunes/yosemite_toads.wav</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>yosemite_toads = pygame.mixer.Sound("/gpio-soundboard/looneytunes/yosemite_toads.wav")</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>btn17.when_pressed = yosemite_toads.play</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>